<commit_message>
Menambahkan Biaya Admin | Fix Selected Dropdown Bulan Pemnbayaran | Menambahkan Popup Transaksi Berhasil
</commit_message>
<xml_diff>
--- a/public/file_export/20210703siswa.xlsx
+++ b/public/file_export/20210703siswa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Muhammad Alghifari</t>
   </si>
@@ -35,58 +35,43 @@
     <t>user</t>
   </si>
   <si>
-    <t>Anwar Ramdhan</t>
-  </si>
-  <si>
-    <t>anwar@gmail.com</t>
-  </si>
-  <si>
-    <t>Unknow</t>
-  </si>
-  <si>
-    <t>0083746356</t>
-  </si>
-  <si>
-    <t>anwar4321</t>
-  </si>
-  <si>
-    <t>Gilang Saputra</t>
-  </si>
-  <si>
-    <t>gilang@gmail.com</t>
-  </si>
-  <si>
-    <t>00837598374</t>
-  </si>
-  <si>
-    <t>gilang4321</t>
-  </si>
-  <si>
-    <t>Raqhin Kusmanadinata</t>
-  </si>
-  <si>
-    <t>raqhin@gmail.com</t>
-  </si>
-  <si>
-    <t>Sanggar Indah Banjaran</t>
-  </si>
-  <si>
-    <t>0047583645</t>
-  </si>
-  <si>
-    <t>raqhin4321</t>
-  </si>
-  <si>
-    <t>Davin Albar</t>
-  </si>
-  <si>
-    <t>davin@gmail.com</t>
-  </si>
-  <si>
-    <t>Sanggar Indah lestari</t>
-  </si>
-  <si>
-    <t>davin4321</t>
+    <t>Nadia Hertisa Isnaeni Putri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hertisanadia44@gmail.com </t>
+  </si>
+  <si>
+    <t>Komplek Permata Kopo C-189</t>
+  </si>
+  <si>
+    <t>0043171547</t>
+  </si>
+  <si>
+    <t>smkn1ktp@01</t>
+  </si>
+  <si>
+    <t>Arianti Apriani Sagita</t>
+  </si>
+  <si>
+    <t>ariantiaprianisagita@gmail.com</t>
+  </si>
+  <si>
+    <t>Kp. Pasanggrahan Rt 02 Rw 06 Kec. Pasirjambu</t>
+  </si>
+  <si>
+    <t>0023620702</t>
+  </si>
+  <si>
+    <t>Ajeng Nurfadillah</t>
+  </si>
+  <si>
+    <t>ajengnurfadilah@gmail.com</t>
+  </si>
+  <si>
+    <t>Jln. Raya Sayuran Rt 08 Rw 07</t>
+  </si>
+  <si>
+    <t>0034169559</t>
   </si>
 </sst>
 </file>
@@ -425,7 +410,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +438,7 @@
         <v>192010521</v>
       </c>
       <c r="G1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1">
         <v>7</v>
@@ -467,7 +452,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -482,10 +467,10 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>193758394</v>
+        <v>192010523</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>7</v>
@@ -499,7 +484,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -508,22 +493,22 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>193758274</v>
+        <v>192010505</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
@@ -531,7 +516,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -546,7 +531,7 @@
         <v>18</v>
       </c>
       <c r="F4">
-        <v>193847568</v>
+        <v>192010501</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -555,41 +540,9 @@
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5">
-        <v>28374658</v>
-      </c>
-      <c r="F5">
-        <v>193748593</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>